<commit_message>
Update information in excel and logs
</commit_message>
<xml_diff>
--- a/app/courses_data.xlsx
+++ b/app/courses_data.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,9 @@
     <col width="27" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,6 +491,21 @@
           <t>Type</t>
         </is>
       </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Number of Modules</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Number of Topics</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -505,6 +523,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -522,6 +551,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -539,6 +579,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -556,6 +607,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -573,6 +635,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -590,6 +663,17 @@
           <t>full-time</t>
         </is>
       </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -607,6 +691,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -624,6 +719,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -641,6 +747,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -658,6 +775,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
@@ -675,6 +803,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -692,6 +831,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -709,6 +859,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -726,6 +887,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>192</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
@@ -743,6 +915,17 @@
           <t>part-time</t>
         </is>
       </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
@@ -759,6 +942,17 @@
         <is>
           <t>part-time</t>
         </is>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update file with logs and excel
</commit_message>
<xml_diff>
--- a/app/courses_data.xlsx
+++ b/app/courses_data.xlsx
@@ -719,7 +719,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти вивчиш базовий синтаксис мови програмування Java. Почнеш знайомство з типами даних та операціями над ними, а вже незабаром ти будеш писати цикли та логічні оператори, які допоможуть тобі розв'язувати базові задачі за допомогою коду. Усе це допоможе тобі на шляху в становленні Java-розробником., Introduction, Main Concepts, Data Types, Operators, Methods, Boolean, Conditionals, Loops, Arrays, String, Practice, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Main Concepts, Data Types, Operators, Methods, Boolean, Conditionals, Loops, Arrays, String, Practice</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Продовжуємо вивчати Java! У цьому модулі ти детальніше розбереш інструменти із Java Basics та виконаєш ще більше практичних завдань!, Type Casting, Arrays Extended, Switch Case, Classes, Classes Advanced, Methods Advanced, Practice</t>
+          <t>Type Casting, Arrays Extended, Switch Case, Classes, Classes Advanced, Methods Advanced, Practice</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -771,8 +771,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Ми хочемо, щоб ви приєдналися до курсу підготовленими і швидко рухалися разом з групою, коли почнеться навчання. 
-Виконання завдань підвищить вашу продуктивність під час курсу і в довгостроковій перспективі допоможе вам отримати роботу в кращій компанії з вищою зарплатою., Intro, Java and IntelliJ Idea, Maven, Checkstyle and Review process</t>
+          <t>Intro, Java and IntelliJ Idea, Maven, Checkstyle and Review process</t>
         </is>
       </c>
     </row>
@@ -789,7 +788,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Ти вже познайомився з основами Java, а зараз ми заглибимося детальніше у світ Java Core. Протягом даного модуля ти дізнаєшся те, що потрібно знати Java-розробнику для того, щоб на співбесідах давати чіткі відповіді та бути впевненим у своїх знаннях. Також ти закріпиш знання на практиці, виконаєш цікаві завдання та реалізуєш власні структури даних. Let’s begin!, How to Solve Tasks, Memory, Wrappers, String, Bit Manipulation, OOP, Abstract Class vs. Interface, Exception, Files, Equals, Hashcode, and Clone, Patterns and Recursion, Generics, ArrayList, LinkedList, PECS, HashMap, Array Practice, Immutable, Set, Queue, Stack, and Comparator, Java JUnit, Java 8 — Part 1, Java 8 — Part 2, Java 8 — Part 3, Java 9-19 Improvements, Stream API Practice, Java SOLID, Java Dependency Injection, Logger</t>
+          <t>How to Solve Tasks, Memory, Wrappers, String, Bit Manipulation, OOP, Abstract Class vs. Interface, Exception, Files, Equals, Hashcode, and Clone, Patterns and Recursion, Generics, ArrayList, LinkedList, PECS, HashMap, Array Practice, Immutable, Set, Queue, Stack, and Comparator, Java JUnit, Java 8 — Part 1, Java 8 — Part 2, Java 8 — Part 3, Java 9-19 Improvements, Stream API Practice, Java SOLID, Java Dependency Injection, Logger</t>
         </is>
       </c>
     </row>
@@ -806,7 +805,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!, Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
         </is>
       </c>
     </row>
@@ -823,7 +822,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>JDBC — це круто, а Hibernate — ще крутіше! Настав час отримати нові знання про взаємодію з базами даних і вийти на новий рівень. У цьому модулі ми подивимося, як «під капотом» працює один із найбільш популярних ORM-фреймворків. Максимум теорії та практики вже чекають на тебе, тож не гаймо часу!, Database Intro, JDBC Intro, Hibernate Entities and Transactions, Entity Relations and Life Cycle, JPA and Cascade Types, Working With Lazy Initialization, Criteria API, Transaction Isolation Levels, N+1 Problem, Database Change Management Tools, SQL Practice, Hibernate Inheritance, Hibernate Cache Levels, Performance Improvement</t>
+          <t>Database Intro, JDBC Intro, Hibernate Entities and Transactions, Entity Relations and Life Cycle, JPA and Cascade Types, Working With Lazy Initialization, Criteria API, Transaction Isolation Levels, N+1 Problem, Database Change Management Tools, SQL Practice, Hibernate Inheritance, Hibernate Cache Levels, Performance Improvement</t>
         </is>
       </c>
     </row>
@@ -881,7 +880,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Розберемо, що воно таке, це IT. Чому IT зараз на хайпі, які типи компаній існують, чим відрізняються та які особливості роботи в кожній із них. Обговоримо ринок ІТ в Україні та як він виживає в сучасних реаліях., General Info About IT, Company Types and UA Market Overview, Non-Tech Roles Overview, Tech Roles Overview, Безкоштовний доступ після реєстрації</t>
+          <t>General Info About IT, Company Types and UA Market Overview, Non-Tech Roles Overview, Tech Roles Overview</t>
         </is>
       </c>
     </row>
@@ -898,7 +897,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Інженери, тестувальники, дизайнери — у чому різниця? Хто всі ці люди? Якими інструментами вони щодня користуються у своїй роботі? Саме це ми й дізнаємось у цьому модулі. А також поговоримо про мови програмування, методології розробки та відмінності між джуніором та сіньором., Software Development Life Cycle, Technologies</t>
+          <t>Software Development Life Cycle, Technologies</t>
         </is>
       </c>
     </row>
@@ -916,8 +915,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Нарешті прийшов час переходити до рекрутмента! Поговоримо про те, як виглядає процес найму в різних компаніях. Навчимося найбільш ефективно взаємодіяти з усіма учасниками процесу рекрутмента, складати опис вакансії та розміщувати її на різних порталах, а також коректно оцінювати подані резюме та писати відгуки.
-І найважливіше — розберемося, що таке етика в рекрутменті та як залишатись професіоналом всупереч зовнішнім обставинам., Recruitment Process Overview, Roles in the Recruitment Process, Vacancy Creation and Posting, Profile Screening</t>
+          <t>Recruitment Process Overview, Roles in the Recruitment Process, Vacancy Creation and Posting, Profile Screening</t>
         </is>
       </c>
     </row>
@@ -934,7 +932,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Не LinkedIn єдиним! Опануємо Boolean Search та X-ray. Будемо шукати ІТ-спеціалістів на GitHub, Stack Overflow, Meetup, Behance та інших профільних ресурсах. Навчимося складати сорсинг-стратегію. Будемо аналізувати профілі кандидатів у соціальних мережах та визначимо, чи варто пропонувати їм вакансію, чи ні. Розберемося в тому, як писати листи кандидатам та на який меседж точно отримаємо відповідь. А ще багато-багато практики!, Boolean Search, X-Ray, LinkedIn, GitHub, Stack Overflow, Kaggle, Dou, Meetup, Other Resources for Sourcing, Mails &amp; Communication, Sourcing Strategy &amp; Candidate Database Management, Sourcing Strategy for CV</t>
+          <t>Boolean Search, X-Ray, LinkedIn, GitHub, Stack Overflow, Kaggle, Dou, Meetup, Other Resources for Sourcing, Mails &amp; Communication, Sourcing Strategy &amp; Candidate Database Management, Sourcing Strategy for CV</t>
         </is>
       </c>
     </row>
@@ -951,7 +949,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу., Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
         </is>
       </c>
     </row>
@@ -968,7 +966,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Як зрозуміти, чи підходите ви один одному? Провести інтерв’ю! Розберемося в різних типах інтерв’ю, оберемо конкретний тип під конкретну ситуацію. Навчимося ставити правильні запитання та аналізувати відповіді. Також поговоримо про фідбек, чому він важливий та як правильно його надавати. А ще прокачаємо свої навички у веденні перемовин, адже перемовини присутні на кожному етапі процесу рекрутмента. Та звичайно, закріпимо це все на практиці!, Interview &amp; Prescreening Structure, Feedback &amp; Job Offer, Recruitment Funnel</t>
+          <t>Interview &amp; Prescreening Structure, Feedback &amp; Job Offer, Recruitment Funnel</t>
         </is>
       </c>
     </row>
@@ -985,7 +983,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому., Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1041,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>На перших порах освоєння дизайну важливо навчитися працювати руками. Розберемося з Figma, дізнаємося про основні UI-компоненти та створимо їх самостійно. Познайомимося з функціоналом Autolayout і Variants. А потім створимо прототип та клікабельний макет мобільного додатка., Figma Essentials, Basic UI Elements, Components, Autolayout, and Variants, Typography Basics, Grids, Prototyping, UI Design, Clickable Prototyping, Безкоштовний доступ після реєстрації</t>
+          <t>Figma Essentials, Basic UI Elements, Components, Autolayout, and Variants, Typography Basics, Grids, Prototyping, UI Design, Clickable Prototyping</t>
         </is>
       </c>
     </row>
@@ -1061,8 +1059,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Ми хочемо, щоб ви приєдналися до курсу підготовленими і швидко рухалися разом з групою, коли почнеться навчання. 
-Ознайомлення з теорією та виконання наведених нижче завдань підвищить вашу продуктивність під час курсу і в довгостроковій перспективі допоможе вам отримати роботу в кращій компанії з вищою заробітною платою., How to learn effectively, Figma practice</t>
+          <t>How to learn effectively, Figma practice</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1076,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Грамотний дизайнер починає з досліджень. Цей модуль присвячений дизайн-процесу роботи над проєктом, коли потрібно дослідити цільову аудиторію та знайти відповіді на безліч питань, перш ніж починати малювати свій макет. Будемо вчитися всім прийомам та створимо власний мобільний додаток., Intro, Design Process, Quantitative Research (Surveys), Heuristic Interface Analysis, Qualitative Research (In-Depth Interviews), Jobs To Be Done, Customer Journey Mapping, Kano Model. Features Prioritization, Information Architecture Mapping, User Flows, Prototyping, Unmoderated User Testing</t>
+          <t>Intro, Design Process, Quantitative Research (Surveys), Heuristic Interface Analysis, Qualitative Research (In-Depth Interviews), Jobs To Be Done, Customer Journey Mapping, Kano Model. Features Prioritization, Information Architecture Mapping, User Flows, Prototyping, Unmoderated User Testing</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1093,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Детально розберемося з фундаментальними принципами та законами візуального дизайну і навчимося використовувати їх в роботі, що в подальшому допоможе тобі створювати якісний UI. Також поглибимо та закріпимо знання UI-елементів, що використовуються в повсякденній роботі., Law of Proximity, Law of Common Region, Negative space, Contrast, Buttons, Inputs</t>
+          <t>Law of Proximity, Law of Common Region, Negative space, Contrast, Buttons, Inputs</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1110,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Коли робота з дослідженням завершена, можна сміливо переходити до «роботи з пікселями» — продумувати зовнішній вигляд макета, розташування та поведінку контенту та багато іншого. У цьому модулі ми доведемо наш додаток до чистового дизайну, готового для передачі в розробку., Grids, Mobile Interfaces, Interface Patterns &amp; Trends, Colors &amp; UI, Typography, Design Gestalts and Rules, Handoff Preparation (UI Kits)</t>
+          <t>Grids, Mobile Interfaces, Interface Patterns &amp; Trends, Colors &amp; UI, Typography, Design Gestalts and Rules, Handoff Preparation (UI Kits)</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1127,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Попрактикуємося в роботі над вебсервісами — навчимося робити дійсно зручні вебінтерфейси та адаптуємо їх. Додамо ще один проєкт у наше портфоліо., Scrum Methodology, Gathering Data From Interviews, Personas and User Stories, Product Hypotheses, Prototyping, Composition and Typography, Graphic Rhymes, Adaptive Design, How to Present Your Work, Project Presentation, Design Systems</t>
+          <t>Scrum Methodology, Gathering Data From Interviews, Personas and User Stories, Product Hypotheses, Prototyping, Composition and Typography, Graphic Rhymes, Adaptive Design, How to Present Your Work, Project Presentation, Design Systems</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1144,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Створимо й оформимо наше портфоліо для Behance. Навчимося цікавим прийомам у роботі над кейсами. Трохи магії, анімації та посидючості — і ми маємо круте портфоліо, з яким сміливо можна шукати роботу., Behance Overview, Case Structure, Trends, Case Design Tips, Second Behance Case</t>
+          <t>Behance Overview, Case Structure, Trends, Case Design Tips, Second Behance Case</t>
         </is>
       </c>
     </row>
@@ -1205,7 +1202,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!, Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
         </is>
       </c>
     </row>
@@ -1223,8 +1220,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Ми хочемо, підготувати тебе до наступних, більш складних  модулів курсу. 
-Ознайомлення з теорією та виконання наведених нижче завдань підвищить вашу продуктивність під час проходження курсу і в довгостроковій перспективі допоможе вам отримати роботу в кращій компанії з вищою заробітною платою., UI elements guide, Course Fundamentals</t>
+          <t>UI elements guide, Course Fundamentals</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1237,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Ще наші предки казали: «Сім раз протестуй — один раз зарелізь». У цьому модулі ми розберемося, що таке тестування, хто за нього відповідає, а також коли воно починається та чому ніколи не закінчується., What is QA, Testing Types, What is a Bug Report, Bug Reports in details, Decomposition, Test Cases, Test Design Techniques, Test Checklist, Software Development Life Cycle, Software Testing Life Cycle, Test Plan, Requirements, TestRail &amp; Jira</t>
+          <t>What is QA, Testing Types, What is a Bug Report, Bug Reports in details, Decomposition, Test Cases, Test Design Techniques, Test Checklist, Software Development Life Cycle, Software Testing Life Cycle, Test Plan, Requirements, TestRail &amp; Jira</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1254,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1271,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Перейдемо до практичних завдань по Git та Terminal., Git and Terminal</t>
+          <t>Git and Terminal</t>
         </is>
       </c>
     </row>
@@ -1292,7 +1288,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Це старт. Тут ти освоїш синтаксис мови JavaScript, ознайомишся зі змінними, циклами, функціями, логічними операторами та іншими базовими конструкціями., Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1305,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS., HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1363,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Починаємо вчити мову програмування Python! У цьому модулі ми познайомимось із синтаксисом, змінними, циклами, функціями, операторами, списками та з іншими базовими конструкціями мови Python., Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary</t>
         </is>
       </c>
     </row>
@@ -1385,8 +1381,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Ми хочемо, підготувати тебе до наступних, більш складних  модулів курсу. 
-Ознайомлення з теорією та виконання наведених нижче завдань підвищить вашу продуктивність під проходження курсу і в довгостроковій перспективі допоможе вам отримати роботу в кращій компанії з вищою заробітною платою., How to learn effectively</t>
+          <t>How to learn effectively</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1398,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Ми вже трохи познайомились із Python. Час продовжити та подивитись детальніше на типи даних, цикли та логічні операції. А також розглянути debugging та code style у Python., Module Overview, Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Lists In Details, Dict Basics, Type Conversion, Loops In Details, Functions Revisited, Summary</t>
+          <t>Module Overview, Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Lists In Details, Dict Basics, Type Conversion, Loops In Details, Functions Revisited, Summary</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1415,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Ми оновили цей модуль. Актуальні теми можна переглянути в Python Basics Extended Upgraded. Ця версія буде видалена 18.08.2024р., Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Functions Revisited, Loops in Details, Type Conversion, Logical Operators, Lists in Details, Dict Basics, Extended Extra</t>
+          <t>Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Functions Revisited, Loops in Details, Type Conversion, Logical Operators, Lists in Details, Dict Basics, Extended Extra</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1432,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -1454,7 +1449,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Ось і настав час заглибитись у світ Python Core і прокачатися як розробник. У цьому модулі ти використаєш знання на практиці, а генератори, ітератори та декоратори перестануть тебе лякати., How to Solve GitHub Tasks, Mutable Immutable Types, List and Dict Comprehensions, Functions in Details, Decorators, Classes, Classes in Details, Iterators and Generators, Modules and Imports, OOP Single Inheritance, OOP Multiple Inheritance, OOP Encapsulation Polymorphism Abstraction, Properties and Descriptors, Exception Handling, Exceptions in Details, File Handling, Memory Management, Testing, Testing in Details, Basic Modules Overview, Dict Advanced, Extra, Python Practice</t>
+          <t>How to Solve GitHub Tasks, Mutable Immutable Types, List and Dict Comprehensions, Functions in Details, Decorators, Classes, Classes in Details, Iterators and Generators, Modules and Imports, OOP Single Inheritance, OOP Multiple Inheritance, OOP Encapsulation Polymorphism Abstraction, Properties and Descriptors, Exception Handling, Exceptions in Details, File Handling, Memory Management, Testing, Testing in Details, Basic Modules Overview, Dict Advanced, Extra, Python Practice</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1466,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!, Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1524,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти познайомишся з основами роботи дата-аналітика, а саме з побудовою візуалізацій. За допомогою сервісу Tableau ти створиш свій перший аналітичний дешборд., Summary, Creating Dashboard, Calculated Fields, Netflix Cinematic Map, Introduction, Безкоштовний доступ після реєстрації</t>
+          <t>Summary, Creating Dashboard, Calculated Fields, Netflix Cinematic Map, Introduction</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1541,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти попрацюєш з електронними таблицями, які використовуються для обчислень, організації, аналізу та зберігання даних. Ти навчишся обробляти датасети, виконувати розрахунки за допомогою функцій та будувати зведені таблиці. Крім того, ти зможеш візуалізувати результати у вигляді графіків та діаграм., Spreadsheet — the Basic Tool for Analytics</t>
+          <t>Spreadsheet — the Basic Tool for Analytics</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1558,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!, Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
         </is>
       </c>
     </row>
@@ -1578,11 +1573,7 @@
           <t>Для роботи дата-аналітика необхідні глибокі знання SQL. Для того, щоб їх отримати, у цьому модулі ти аналізуватимеш показники продажів і маркетингу на основі реальної бази даних, що містить дані з інтернет-магазину.</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Для роботи дата-аналітика необхідні глибокі знання SQL. Для того, щоб їх отримати, у цьому модулі ти аналізуватимеш показники продажів і маркетингу на основі реальної бази даних, що містить дані з інтернет-магазину.</t>
-        </is>
-      </c>
+      <c r="C5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1597,7 +1588,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Починаємо вчити мову програмування Python! У цьому модулі ми познайомимось із синтаксисом, змінними, циклами, функціями, операторами, списками та з іншими базовими конструкціями мови Python., Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary</t>
         </is>
       </c>
     </row>
@@ -1612,11 +1603,7 @@
           <t>Python — надзвичайно потужний інструмент для дата аналізу. Ти вже вивчив основи, то ж ми переходимо до ознайомлення з бібліотеками NumPy та Pandas для обробки та аналізу даних. Також ти навчишся візуалізувати результати за допомогою Matplotlib та Seaborn та працювати з інтерактивними середовищами, такими як Jupyter Notebooks та Google Colab, для виконання та документування своїх аналітичних задач.</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>Python — надзвичайно потужний інструмент для дата аналізу. Ти вже вивчив основи, то ж ми переходимо до ознайомлення з бібліотеками NumPy та Pandas для обробки та аналізу даних. Також ти навчишся візуалізувати результати за допомогою Matplotlib та Seaborn та працювати з інтерактивними середовищами, такими як Jupyter Notebooks та Google Colab, для виконання та документування своїх аналітичних задач.</t>
-        </is>
-      </c>
+      <c r="C7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -1629,11 +1616,7 @@
           <t>Tableau — це ціла екосистема інтерактивної аналітики. У цьому модулі ти навчишся підключати дані та створювати комбіновані джерела даних, робити складні візуалізації, публікувати та оновлювати дешборди. Також ти навчишся використовувати  Tableau Prep для підготовки даних, та Tableau Public і Tableau Online для спільного доступу до своїх робіт.</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Tableau — це ціла екосистема інтерактивної аналітики. У цьому модулі ти навчишся підключати дані та створювати комбіновані джерела даних, робити складні візуалізації, публікувати та оновлювати дешборди. Також ти навчишся використовувати  Tableau Prep для підготовки даних, та Tableau Public і Tableau Online для спільного доступу до своїх робіт.</t>
-        </is>
-      </c>
+      <c r="C8" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1689,7 +1672,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Це твій старт в digital marketing! Тут ти вивчиш основи маркетингу та дізнаєшся про його цілі, познайомишся з каналами та джерелами офлайн-маркетингу та онлайн-маркетингу, дізнаєшся про їх переваги та недоліки., Marketing Introduction, Offline Marketing vs. Online Marketing, Google Ads Search, Keywords, Your First Media Plan, Growth Opportunities, Course Overview, Безкоштовний доступ після реєстрації</t>
+          <t>Marketing Introduction, Offline Marketing vs. Online Marketing, Google Ads Search, Keywords, Your First Media Plan, Growth Opportunities, Course Overview</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1689,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти навчишся досліджувати ринок та розуміти потенційну вигоду від виходу твого продукту на новий ринок.  Також відкриєш для себе відповіді на питання про об'єми ринку, одержиш інформацію про твоїх ключових конкурентів та побудуєш точки диференціації від них. А ще навчишся описувати профіль потенційного клієнта, враховуючи його «болі», а також зрозумієш як правильно описувати продукт або сервіс, щоб розмовляти з клієнтом «однією мовою»., Market Sizing, Competitors Analysis, Customer Portrait, Points of Differentiation, Value Proposition</t>
+          <t>Market Sizing, Competitors Analysis, Customer Portrait, Points of Differentiation, Value Proposition</t>
         </is>
       </c>
     </row>
@@ -1723,7 +1706,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Головна мета маркетингу — продажі. У цьому модулі ти познайомишся з інструментом, який надає найшвидші результати для досягнення цієї мети! Ти у деталях оглянеш Google Ads та його можливості. А ще налаштуєш свою першу рекламну кампанію, обравши релевантні цілі та типи. Також навчишся розуміти як різні типи кампаній впливають на досягнення цілей. І наостанок — створиш перше оголошення на пошуку та навчишся оптимізувати рекламні кампанії для пошуку., Google Ads Set Up, Campaign Structure, Campaign Objectives, Conversions, Campaign Types, Creating an Ad, Additional Settings of Google Ads Campaigns, Google Search Optimization</t>
+          <t>Google Ads Set Up, Campaign Structure, Campaign Objectives, Conversions, Campaign Types, Creating an Ad, Additional Settings of Google Ads Campaigns, Google Search Optimization</t>
         </is>
       </c>
     </row>
@@ -1740,7 +1723,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти розглянеш ще один важливий маркетинговий інструмент – Google Display Network (GDN) та YouTube. Ти отримаєш розуміння про те, як працює GDN і як його ефективно використовувати, налаштуєш свою першу рекламну кампанію на GDN, зрозумієш як правильно таргетувати  та оптимізувати GDN оголошення, познайомишся з додатковими налаштуваннями GDN. Ще ми розглянемо як аналізувати ефективність рекламних кампаній та як приймати на їх основі обґрунтовані рішення для подальшого розвитку., Campaign Creation, Targeting, Ads Creation, Google Display Ads Optimization</t>
+          <t>Campaign Creation, Targeting, Ads Creation, Google Display Ads Optimization</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1740,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Тут ти познайомишся зі ще одним рекламним інструментом — Meta Ads. А також: розберешся з принципами роботи таргетованої реклами у соціальних мережах на кейсах з Facebook та Instagram, проаналізуєш актуальні алгоритми, створиш та налаштуєш свій рекламний кабінет Meta, протестуєш основні типи оптимізації, створюючи рекламні кампанії та рекламні оголошення!, Meta Ads Overview, Meta Ads Setup, Meta Audience Types, Campaign Objectives, How to create Meta Ad Campaign, Creatives. Ad formats, Optimization of Advertising Campaigns</t>
+          <t>Meta Ads Overview, Meta Ads Setup, Meta Audience Types, Campaign Objectives, How to create Meta Ad Campaign, Creatives. Ad formats, Optimization of Advertising Campaigns</t>
         </is>
       </c>
     </row>
@@ -1774,7 +1757,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Тепер поговоримо про важливість та можливості SEO у digital-маркетингу. Зосередимось на ранжуванні сторінок, створенні кластерів для пошукових запитів, побудові посилань, а також розрізненні методів просування.Ти навчишся виконувати аудит сайтів, зрозумієш семантику, внутрішню та зовнішню оптимізацію, розберешся в принципах роботи пошукових систем та санкціях Google, а також опануєш інструменти відстеження результатів (Google Analytics, Google Search Console тощо)., Introduction to SEO, Working with Keywords, On-Page Optimization, Working with Content, Link Building, What's Next?, Competitor Analysis</t>
+          <t>Introduction to SEO, Working with Keywords, On-Page Optimization, Working with Content, Link Building, What's Next?, Competitor Analysis</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1774,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ми познайомимось та навчимось користуватись різноманітними Brand Awareness каналами, зокрема такими як PR, SMM, Content Marketing, Influence Marketing та Event Marketing. Навчимось шукати та аналізувати медіа-ресурси, створювати ефективні контент-плани, підбирати релевантні інструменти, які підходять саме для твого бізнесу. Відкриємо для себе можливості Outbound Lead Generation, навчимось створювати та аналізувати ефективність cold emails, розглянемо стратегії комунікації через LinkedIn, зрозуміємо де доцільно використовувати ABM (Account-Based Marketing). Також ми навчимось створювати та автоматизовувати ефективні email-кампанії, програми лояльності та реферальні програми., Brand Awareness Channels, Outbound Lead Generation, Customer Activation, Portfolio Project, Customer Loyalty and Referral Programs</t>
+          <t>Brand Awareness Channels, Outbound Lead Generation, Customer Activation, Portfolio Project, Customer Loyalty and Referral Programs</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1832,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Це старт. Тут ти освоїш синтаксис мови JavaScript, ознайомишся зі змінними, циклами, функціями, логічними операторами та іншими базовими конструкціями., Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1849,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>В цьому модулі зібрані інформація, поради та завдання, які допоможуть тобі більш ефективно навчатися на курсі, а в довгостроковій перспективі отримати роботу в кращій компанії з вищою заробітною платою., Environment Setup, How to Learn Effectively</t>
+          <t>Environment Setup, How to Learn Effectively</t>
         </is>
       </c>
     </row>
@@ -1883,7 +1866,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS., HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
         </is>
       </c>
     </row>
@@ -1900,7 +1883,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1900,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Продовжимо знайомство з JavaScript? Час подивитися на рядки, числа та цикли з іншої сторони. Ох, а об'єкти чого тільки варті ... І на десерт — ще порція задач для додаткової практики!, Code Style, Working With Numbers, Loops in Details, Working With Strings, Functions Revisited, Switch, Type Conversion, Logical Operators, Object Basics, Extended Extra</t>
+          <t>Code Style, Working With Numbers, Loops in Details, Working With Strings, Functions Revisited, Switch, Type Conversion, Logical Operators, Object Basics, Extended Extra</t>
         </is>
       </c>
     </row>
@@ -1934,7 +1917,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Верстають усі! У цьому модулі ти поглибиш свої знання у верстці, розберешся з псевдокласами, псевдоелементами, розглянеш основи препроцесора Sass, а також познайомишся з методологією BEM. Ну і в якості вишеньки на тортику — зверстаєш лендінг для свого портфоліо!, Environment Setup, Flexbox, BEM, Sass, Transformations and Animations, Grid, Landing [Portfolio Project], Document and Events</t>
+          <t>Environment Setup, Flexbox, BEM, Sass, Transformations and Animations, Grid, Landing [Portfolio Project], Document and Events</t>
         </is>
       </c>
     </row>
@@ -1951,7 +1934,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Тепер поглибимо наші знання та закріпимо базу на практиці. Навчимося працювати з GitHub та отримаємо зворотній зв'язок від менторів на написаний код. Навчимося робити інтерфейси не тільки гарними, але й функціональними! Зробимо перший запит на сервер та багато-багато іншого!, How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
+          <t>How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
         </is>
       </c>
     </row>
@@ -2009,7 +1992,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Це старт. Тут ти освоїш синтаксис мови JavaScript, ознайомишся зі змінними, циклами, функціями, логічними операторами та іншими базовими конструкціями., Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview</t>
         </is>
       </c>
     </row>
@@ -2026,7 +2009,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>В цьому модулі зібрані інформація, поради та завдання, які допоможуть тобі більш ефективно навчатися на курсі, а в довгостроковій перспективі отримати роботу в кращій компанії з вищою заробітною платою., How to Learn Effectively, Environment Setup</t>
+          <t>How to Learn Effectively, Environment Setup</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2026,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS., HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
         </is>
       </c>
     </row>
@@ -2060,7 +2043,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2060,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Продовжимо знайомство з JavaScript? Час подивитися на рядки, числа та цикли з іншої сторони. Ох, а об'єкти чого тільки варті ... І на десерт — ще порція задач для додаткової практики!, Code Style, Working With Numbers, Loops in Details, Working With Strings, Functions Revisited, Switch, Type Conversion, Logical Operators, Object Basics, Extended Extra</t>
+          <t>Code Style, Working With Numbers, Loops in Details, Working With Strings, Functions Revisited, Switch, Type Conversion, Logical Operators, Object Basics, Extended Extra</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2077,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Верстають усі! У цьому модулі ти поглибиш свої знання у верстці, розберешся з псевдокласами, псевдоелементами, розглянеш основи препроцесора Sass, а також познайомишся з методологією BEM. Ну і в якості вишеньки на тортику — зверстаєш лендінг для свого портфоліо!, Environment Setup, Flexbox, BEM, Sass, Transformations and Animations, Grid, Landing [Portfolio Project], Document and Events</t>
+          <t>Environment Setup, Flexbox, BEM, Sass, Transformations and Animations, Grid, Landing [Portfolio Project], Document and Events</t>
         </is>
       </c>
     </row>
@@ -2111,7 +2094,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Тепер поглибимо наші знання та закріпимо базу на практиці. Навчимося працювати з GitHub та отримаємо зворотній зв'язок від менторів на написаний код. Навчимося робити інтерфейси не тільки гарними, але й функціональними! Зробимо перший запит на сервер та багато-багато іншого!, How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
+          <t>How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2152,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Починаємо вчити мову програмування Python! У цьому модулі ми познайомимось із синтаксисом, змінними, циклами, функціями, операторами, списками та з іншими базовими конструкціями мови Python., Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary, Безкоштовний доступ після реєстрації</t>
+          <t>Introduction, Main Concepts, Numbers, Strings, Boolean, Lists, Conditional Operators, Loops, Functions, Summary</t>
         </is>
       </c>
     </row>
@@ -2186,7 +2169,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Ми вже трохи познайомились із Python. Час продовжити та подивитись детальніше на типи даних, цикли та логічні операції. А також розглянути debugging та code style у Python., Module Overview, Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Lists In Details, Dict Basics, Type Conversion, Loops In Details, Functions Revisited, Summary</t>
+          <t>Module Overview, Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Lists In Details, Dict Basics, Type Conversion, Loops In Details, Functions Revisited, Summary</t>
         </is>
       </c>
     </row>
@@ -2203,7 +2186,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Ми оновили цей модуль. Актуальні теми можна переглянути в Python Basics Extended Upgraded. Ця версія буде видалена 18.08.2024р., Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Functions Revisited, Loops in Details, Type Conversion, Logical Operators, Lists in Details, Dict Basics, Extended Extra</t>
+          <t>Environment Setup, Code Style, Debugging, Working With Numbers, Working With Strings, Functions Revisited, Loops in Details, Type Conversion, Logical Operators, Lists in Details, Dict Basics, Extended Extra</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2203,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Термінал — один з основних інструментів будь-якого розробника. У цьому модулі ти познайомишся із базовими командами термінала, а також дізнаєшся, що таке система контролю версій Git та як нею користуватися., Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
+          <t>Environment Setup, Command Line Basics, Git Basics, Working With Branches, Working With Remote Repo (GitHub)</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2220,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>У цьому модулі ти розглянеш як організована розробка програмного забезпечення та як її можна оптимізувати. А найголовніше — яка роль DevOps-інженера в усьому цьому., Introduction, DevOps Culture and Practices, DevOps as a Role, SDLC and Development Methodologies, Summary</t>
+          <t>Introduction, DevOps Culture and Practices, DevOps as a Role, SDLC and Development Methodologies, Summary</t>
         </is>
       </c>
     </row>
@@ -2254,7 +2237,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому., Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
         </is>
       </c>
     </row>
@@ -2271,7 +2254,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Що спільного у твого ноутбука, мобільного телефону та хмарного сервера? Це все комп’ютери під керуванням певної операційної системи. У цьому модулі ми розглянемо основи роботи з ОС та серверами, наприклад, Ubuntu та NGINX., Environment Setup, What Is Operating System, Working With Files, Processes and Services, Resource Management, Managing Users, Installing Software, Using SSH, Shell Scripting, Web Server</t>
+          <t>Environment Setup, What Is Operating System, Working With Files, Processes and Services, Resource Management, Managing Users, Installing Software, Using SSH, Shell Scripting, Web Server</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update logs and excel files
</commit_message>
<xml_diff>
--- a/app/courses_data.xlsx
+++ b/app/courses_data.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,10 @@
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,6 +486,26 @@
           <t>Description</t>
         </is>
       </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Number of Modules</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Number of Topics</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Full-Time Duration</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Part-Time Duration</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -499,6 +523,22 @@
           <t>UI/UX-дизайнери спеціалізуються на інтерфейсах додатків. Вони враховують потреби користувачів, їх взаємодії з продуктом та створюють зручний, естетичний та зрозумілий дизайн, який відповідає цим потребам.</t>
         </is>
       </c>
+      <c r="D2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -516,6 +556,22 @@
           <t>QA-інженер відповідає за розробку планів тестування додатків та сайтів. Тестувальник виявляє недоліки в роботі продукту, а що найважливіше — допомагає уникнути їх у майбутньому.</t>
         </is>
       </c>
+      <c r="D3" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>148</v>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -533,6 +589,22 @@
           <t>Python-розробники можуть працювати в різних сферах: від машинного навчання до веброзробки. Вони володіють знаннями, необхідними для створення, розширення та підтримки програм, які використовують Python як основну мову програмування.</t>
         </is>
       </c>
+      <c r="D4" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>185</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -550,6 +622,22 @@
           <t>Він допомагає бізнесу приймати рішення на основі даних. Такий підхід дозволяє компаніям розуміти попит на свої продукти, збільшувати продажі, а також краще задовольняти потреби клієнтів.</t>
         </is>
       </c>
+      <c r="D5" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -567,6 +655,22 @@
           <t>Використовуй різноманітні маркетингові стратегії, соціальні мережі, пошуковий маркетинг, контент-маркетинг та інші інструменти, щоб рекламувати бренди та залучати цільову аудиторію.</t>
         </is>
       </c>
+      <c r="D6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -584,6 +688,22 @@
           <t>Frontend-розробник відповідає за створення зручного та естетичного вигляду вебсторінки на різних пристроях, а також реалізує анімації та інші інтерфейсні рішення.</t>
         </is>
       </c>
+      <c r="D7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>138</v>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -601,6 +721,22 @@
           <t>Fullstack-розробники володіють навичками програмування як фронтенду (клієнтська сторона), так і бекенду (серверна сторона). Вони можуть розробити повноцінний продукт від початку до кінця.</t>
         </is>
       </c>
+      <c r="D8" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>182</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -618,6 +754,22 @@
           <t>DevOps-інженер відповідає за ефективний процес створення програмного продукту, а також виявляє шляхи автоматизації процесів розробки, забезпечуючи надійне та ефективне постачання продукту до кінцевого користувача.</t>
         </is>
       </c>
+      <c r="D9" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>192</v>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -635,6 +787,22 @@
           <t>Java-розробники — це творці потужних та надійних додатків, які застосовуються в різних сферах, від роботи банків до агросектору.</t>
         </is>
       </c>
+      <c r="D10" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>166</v>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -650,6 +818,22 @@
       <c r="C11" s="3" t="inlineStr">
         <is>
           <t>IT-рекрутери забезпечують розвиток команд. Це експерти у галузі знаходження та відбору кандидатів для вакансій, пов'язаних із розробкою програмного забезпечення, базами даних та іншими IT-напрямками.</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
         </is>
       </c>
     </row>
@@ -676,7 +860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,7 +868,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="32" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -823,6 +1007,159 @@
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>Database Intro, JDBC Intro, Hibernate Entities and Transactions, Entity Relations and Life Cycle, JPA and Cascade Types, Working With Lazy Initialization, Criteria API, Transaction Isolation Levels, N+1 Problem, Database Change Management Tools, SQL Practice, Hibernate Inheritance, Hibernate Cache Levels, Performance Improvement</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>How the Web Works</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Spring Boot</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Spring Boot — це як Spring, але зовсім іншого рівня! Більше не потрібно вручну налаштовувати вебсервер, підключення до бази даних або залежності для проєкту. Spring Boot попіклується про це, щоб ти сконцентрувався на більш важливих речах — створенні логіки додатка. Протягом цього модуля ти дізнаєшся, як користуватися Spring Boot, як він працює «під капотом» та які «плюшки» пропонує.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Spring Boot Intro, Spring Bean Lifecycle, Spring Boot Web, Spring Boot Web: DTO, Spring Boot Web: Mappers in Details, Spring Data JPA, Criteria Query in Spring Boot, Spring Transactional, GlobalExceptionHandler and Data Validation, Pagination, Sorting, Swagger, Working With Third-Party API, Security Basics, Spring Boot Security, JWT, Spring Boot Practice, Docker in Spring Boot, Spring Boot Testing, Deploy the Project to AWS, Spring Boot AOP, Portfolio Project</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Java Multithreading</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Багатопоточність допомагає швидше та ефективніше працювати з великою кількістю даних, а також більш ефективно використовувати ресурс процесора. Щоб навчитися працювати з таким часто непередбачуваним інструментом, потрібна уважність до деталей, та воно того варте! У цьому модулі ти розглянеш основний синтаксис для роботи в багатопоточному режимі, а також розповсюджені класи та інтерфейси для вирішення основних завдань.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Multithreading intro, Threads, JMM (Java Memory Model), Thread manipulation, Locks, Deadlock, ExecutorService and Future, CompletableFuture, Concurrent collections</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Kotlin</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Пориньте у захоплюючий світ розробки додатків для Android за допомогою нашого модуля Kotlin! Вивчіть основи цієї інноваційної мови та зробіть свій перший крок до створення передових програм для Android.</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Kotlin Intro, Variables, Data Types, and Operators, Nullability, Functions, Collections, Conditionals, and Loops, Classes (OOP), Classes (Advanced), Extensions, Exceptions and Files, Standard Functions and Other Concepts</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Алгоритми замовляли? У цьому модулі ми познайомимося з різними структурами даних та алгоритмами. Навчимося обходити дерева краще сина маминої подруги, сортувати масиви зі швидкістю quick sort, створювати hash map та не тільки стояти в черзі, а й реалізовувати її. І це тільки маленька частинка того, що тебе чекає в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, Algorithm Complexity, Data Structures: Array, Search Algorithms, Data Structures: Linked List, Data Structures: Stack, Data Structures: Queue, Data Structures: Hash Map, Data Structures: Hash Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>HTML + CSS Basics</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS.</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Angular</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Angular — це популярний JS-фреймворк для створення масштабованих односторінкових вебдодатків. У цьому модулі ти вивчиш концепції Angular, від основ і структури проєкту до складних тем, таких як форми, компоненти, спостережувані параметри, управління станом, обробка помилок і оптимізація продуктивності.</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Angular Basics</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
         </is>
       </c>
     </row>
@@ -837,7 +1174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -987,6 +1324,23 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -998,7 +1352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1148,6 +1502,74 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Creative Web</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Цілковито зануримось в роботу з UI і створимо нестандартний концепт веб-сайту, який згодом оформимо у ще один проєкт для портфоліо. На тебе чекає багато практики та експериментів з композицією, типографією, кольорами й іншим візуальним контентом.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Design exploration, Site structure and mood board, Wireframing, Concept creation, Adapting design, Third Behance case</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>HTML + CSS Basics</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1159,7 +1581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1167,7 +1589,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="29" customWidth="1" min="1" max="1"/>
+    <col width="38" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -1306,6 +1728,210 @@
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript Basics Extended</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Продовжимо знайомство з JavaScript? Час подивитися на рядки, числа та цикли з іншої сторони. Ох, а об'єкти чого тільки варті ... І на десерт — ще порція задач для додаткової практики!</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Code Style, Working With Numbers, Loops in Details, Working With Strings, Functions Revisited, Switch, Type Conversion, Logical Operators, Object Basics, Extended Extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>How the Web Works</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Testing Web Applications</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Чому QA має знати, як працює Інтернет? Питання, яке хвилювало багатьох грецьких філософів (якби в їх часи був Інтернет). У цьому модулі ми дізнаємося про те, що приховано під шаром GUI браузера, як з цим має працювати QA та які інструменти можуть допомогти підвищити ефективність тестування.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Browser DevTools, Web Theory and Postman Basics, Postman Advanced</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Mobile testing</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Що будить більшість людей зранку і яку річ майже кожен з нас тримає в руках перед сном? На початку 2000-х відповідь була не такою очевидною, але в наші дні мобільні пристрої повсюди, і для кожного з них потрібні десятки додатків, які треба протестувати. Але як?</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Mobile testing theory, Guidelines, Mobile testing activities, Emulators and Tools</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Working With Infrastructure</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Що таке тестове середовище? Які існують середовища для тестування? Як налаштувати локальний сервер і як підключитися до локальної бази даних? Спробуємо розібратися.</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Working Environments, SQL, Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>QA Ethics</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Ми майже готові почати працевлаштування, але які каверзні запитання про QA можуть бути на нашому шляху до омріяного оферу? Обговоримо деякі з них, а також поговоримо про те, як спілкуватися з товаришами по команді так, щоб вас не звільнили наступного дня.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Interview Questions, QA Ethics</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript Advanced</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Тепер поглибимо наші знання та закріпимо базу на практиці. Навчимося працювати з GitHub та отримаємо зворотній зв'язок від менторів на написаний код. Навчимося робити інтерфейси не тільки гарними, але й функціональними! Зробимо перший запит на сервер та багато-багато іншого!</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript Testing</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Тестування — це важливо! Але чим більше коду, тим більше треба перевіряти кожного разу. Автоматизація дозволить значно спростити цей процес.</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to Javascript Automated Testing, Unit Testing, TDD Basics, Mock Basics, Advanced Mocks, Cypress</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Application Testing on macOS</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль охоплює особливості екосистеми macOS, інструменти для пошуку помилок і дебаггінгу, UI-тестування згідно з Apple Human Interface Guidelines, продуктову аналітику та автоматизоване тестування.</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, macOS Fundamentals, macOS Version History, Basics of Testing Apps on macOS, Process and Memory Management, Daemons and Agents, Permissions in macOS, Sandbox, System Integrity Protocol, Gatekeeper, Network Utilities and Diagnostics, Testing GUI &amp; UX, Product Analytics Testing, Introduction to Test Automation for macOS Apps</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Алгоритми замовляли? У цьому модулі ми познайомимося з різними структурами даних та алгоритмами. Навчимося обходити дерева краще сина маминої подруги, сортувати масиви зі швидкістю quick sort, створювати hash map та не тільки стояти в черзі, а й реалізовувати її. І це тільки маленька частинка того, що тебе чекає в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, Algorithm Complexity, Data Structures: Array, Search Algorithms, Data Structures: Linked List, Data Structures: Stack, Data Structures: Queue, Data Structures: Hash Map, Data Structures: Hash Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1470,6 +2096,211 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Django ORM</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>У цьому розділі ти познайомишся з однією з найпопулярніших ORM для роботи з базами даних на Python. Ти навчишся створювати таблиці та робити прості та складні SQL-запити за допомогою інтерфейсу Django ORM. А головне — цей модуль підготує тебе до знайомства із Django!</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Database Intro, ORM Intro, Fields and Relations, Many-to-Many Relationship, Queries, Queries in Details, ORM Advanced, Optional: Performance Improvement &amp; Isolation Levels</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>HTML + CSS Basics</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Поверстаємо? В цьому модулі ти ознайомишся з базовими конструкціями мови розмітки HTML та мовою стилів CSS.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>HTML Basics, CSS Basics, Colors and Fonts, Box Model Basics, Semantic Basics, Responsiveness Basics, CSS Selectors, Pseudo-Elements and Pseudo-Classes, Specificity, Links and URLs, Images, Media Queries, Forms, Position, Extra Topics</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>How the Web Works</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Django</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Нарешті ми дійшли до найпопулярнішого вебфреймворку в  Python — Django. MVT, Dependency Injection, Web — тепер будуть у твоєму розпорядженні. Тут ти попрактикуєш HTML та CSS, а також попрацюєш із базами даних та отримаєш навички, які точно знадобляться тобі в майбутніх проєктах.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Django Intro, MVT, Class-Based Generic Views, Sessions and Authentication, Forms, Forms in Details, Django Advanced, Website [Portfolio Project], Deploying Django, Django Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Django REST Framework</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Якщо ти хочеш розробляти потужні API, то Django REST Framework — 100% твій вибір. У цьому модулі ти попрактикуєшся в написанні API, дізнаєшся, як проходить процес аутентифікації користувачів, та протестуєш власний написаний код. Пориньмо у світ Python Backend!</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Django REST Framework Intro, Class-Based Views, Serializers, Serializers in Details, Authentication &amp; Permissions, Django REST Framework Advanced, DRF JWT and Tests, Docker, Docker in DRF, API [Portfolio Project], Test Task Solving, Connect Backend to Frontend, DRF Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Asynchronous Python</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Набридло все робити крок за кроком, рядок за рядком? Тоді цей модуль саме для тебе! Тут ти навчишся пришвидшувати роботу програми завдяки асинхронності та розберешся із поняттями конкурентності та паралелізму.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Concurrency &amp; Parallelism, Asyncio</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Object Oriented Programming</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>На технічній співбесіді початківців часто запитують про Об'єктно-орієнтоване програмування (ООП) та його основні принципи.
+У цьомо модулі ти познайомишся з основами ООП та іншими речами, про які тебе можуть запитати.</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Basic Principles, SOLID Principles</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Python Advanced</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Ще більше Python! У цьому модулі ми розглянемо складніші приклади: пропарсимо вебсторінку, проаналізуємо дані, навчимось будувати графіки та навіть створимо власну модель для машинного навчання!</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>SOLID Practice, FastAPI overview, FastAPI in details, Web Scraping, Selenium, Scrapy, Data Analysis, Pandas &amp; Matplotlib, ETL &amp; Visualising Practice, [Portfolio Project]: Web Scraping &amp; Data Analysis Practice, Tableau, Machine Learning, Neural Networks &amp; Classification, Machine Learning Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Алгоритми замовляли? У цьому модулі ми познайомимося з різними структурами даних та алгоритмами. Навчимося обходити дерева краще сина маминої подруги, сортувати масиви зі швидкістю quick sort, створювати hash map та не тільки стояти в черзі, а й реалізовувати її. І це тільки маленька частинка того, що тебе чекає в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, Algorithm Complexity, Data Structures: Array, Search Algorithms, Data Structures: Linked List, Data Structures: Stack, Data Structures: Queue, Data Structures: Hash Map, Data Structures: Hash Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript Basics</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Це старт. Тут ти освоїш синтаксис мови JavaScript, ознайомишся зі змінними, циклами, функціями, логічними операторами та іншими базовими конструкціями.</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Your First JavaScript Program, Main Concepts, Numbers, Strings, Boolean, Functions, Conditional Operators, Arrays, Loops, String Iteration, Strings Methods, Working With Arrays, Get Ready for the Interview</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1481,7 +2312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1489,7 +2320,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -1617,6 +2448,75 @@
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Статистика — тема непроста, але ми постаралися зібрати тільки ту інформацію, яка знадобиться тобі для виконання реальних робочих задач дата аналітика. У цьому модулі ти навчишся основам статистики, включаючи її роль у бізнесі та повсякденному житті. Також ти попрацюєш над аналізом взаємозвʼязків між даними, перевіркою гіпотез та навчишся дизайну статистичних експериментів.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Product A/B Testing</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Починаємо формувати продуктове мислення. У цьому модулі ти навчишся підходам до оцінки гіпотез, зокрема A/B tests. Ти дізнаєшся, як будувати продуктові гіпотези, розробляти дизайн A/B тестів, обирати метрики для їх проведення та аналізувати результати.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Product and Marketing Metrics</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Продовжуємо розвивати продуктове мислення. У цьому модулі ти навчишся оцінювати залучення користувачів, аналізувати активацію та утримання. Ти освоїш типові продуктові фреймворки, такі як когортний аналіз, RFM, NSM, та ARRR. Крім того, ти створиш карту метрик для сайту в якості проєкту.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Advanced Analytics: Prediction and Clustering Models</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Занурюємося в аналітику. У цьому модулі ти навчишся прогнозуванню кількісних показників за допомогою лінійної багатофакторної моделі та лінійної регресійної моделі з однією пояснюючою змінною. Ти освоїш поняття тренувальних і тестових даних, крос-валідацію, міри якості моделі, регуляризацію, а також прогнозування якісних показників і ризиків за допомогою логістичної регресії. Крім того, ти дізнаєшся про кластерний аналіз, методи кластеризації даних, міри схожості та алгоритми, такі як k-середніх, k-медіан та DBSCAN.</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1629,7 +2529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1778,6 +2678,40 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Digital Marketing Analytics</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти дізнаєшся як правильно робити аналіз, щоб оцінювати ефективність digital-маркетингу та коригувати стратегію. Ми розберемось з ключовими інструментами та сервісами для аналітики, познайомимось з Google Analytics та зробимо базові налаштування. Також ми розглянемо інтерфейс основних звітів, та поговоримо про кастомні звіти. Наприкінці модуля ти зрозумієш як обрати та впровадити ключові інструменти та сервіси для аналітики для свого бізнесу, а також зрозумієш, як формувати основні звіти.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Social Media Analytics, Web Analytics, Paid Advertising Analytics, Metrics of Effectiveness, Reporting and Analysis, DM Analytics Overview, CRM Analytics, Email Marketing Analytics</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1789,7 +2723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1797,7 +2731,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="32" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -1935,6 +2869,228 @@
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>DOM, Events, Promises</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>В цьому модулі ти дізнаєшся як керувати сторінкою за допомогою JavaScript, а також про асинхронність у JavaScript.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>DOM Basics, DOM Styling and Sizing, Events, Promises, Portfolio Project</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>React</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Реактивненько вриваємось у світ фреймворків та UI-бібліотек. Прийшов час познайомитися з однією з найпопулярніших бібліотек у фронтенд-розробці. У цьому модулі ти дізнаєшся, що таке компонентний підхід до розробки, а також розробиш перший інтерактивний інтерфейс та створиш роботу для портфоліо!</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Props, Rendering Lists, Handling Events, List Manipulation, Lifting State Up, Updating State</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>TypeScript</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript ми вже знаємо. Прийшла черга зробити наш код більш передбачуваним і безпечним, а розробку приємнішою. У цьому модулі ти дізнаєшся, що таке статична типізація й чим корисний TypeScript для розробника.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Basic Types, Advanced Types, Object Types, Classes, Generic Types</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>React with TypeScript</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти познайомишся з магією TypeScript у React.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Forms, Advanced Hooks, Component Lifecycle, Custom Hooks, Loading Data From API, Updating Data on Server, State Management, React Router, Working With URLSearchParams, Portfolio</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Redux</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Що там по менеджменту? Розберемось, як використовувати бібліотеку Redux в парі з бібліотекою React для менеджменту загального стану твого додатка. Припинимо прокидатися в холодному поту від слова «ред'юсер». Або почнемо…</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, React Redux, Async Redux</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>How the Web Works</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Tech Interview</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ми розглянемо важливі теми для проходження технічної співбесіди, які залишилися поза курсом.</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Final Portfolio Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Vue.js</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти створиш додаток ToDo за допомогою фреймворку Vue.js, використовуючи його систему реактивності, компоненти та обробку даних за допомогою Axios. Ти також вивчиш передові методи та розгорнеш свій додаток на GitHub Pages.</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>TodoApp with Vue.js</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Angular</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Angular — це популярний JS-фреймворк для створення масштабованих односторінкових вебдодатків. У цьому модулі ти вивчиш концепції Angular, від основ і структури проєкту до складних тем, таких як форми, компоненти, спостережувані параметри, управління станом, обробка помилок і оптимізація продуктивності.</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Angular Basics</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Алгоритми замовляли? У цьому модулі ми познайомимося з різними структурами даних та алгоритмами. Навчимося обходити дерева краще сина маминої подруги, сортувати масиви зі швидкістю quick sort, створювати hash map та не тільки стояти в черзі, а й реалізовувати її. І це тільки маленька частинка того, що тебе чекає в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, Algorithm Complexity, Data Structures: Array, Search Algorithms, Data Structures: Linked List, Data Structures: Stack, Data Structures: Queue, Data Structures: Hash Map, Data Structures: Hash Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Object Oriented Programming</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>На технічній співбесіді початківців часто запитують про Об'єктно-орієнтоване програмування (ООП) та його основні принципи.
+У цьомо модулі ти познайомишся з основами ООП та іншими речами, про які тебе можуть запитати.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Basic Principles, SOLID Principles</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
         </is>
       </c>
     </row>
@@ -1949,7 +3105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1957,7 +3113,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="32" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -2095,6 +3251,313 @@
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>How to Solve Tasks on Github, Object Advanced, Methods, Array Methods, Callbacks, Array Iteration Methods Implementation, Array Iteration Methods Usage, Array Iteration Methods Practice, Closures, JS Practice, Prototype, Constructors, Classes, Extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>DOM, Events, Promises</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>В цьому модулі ти дізнаєшся як керувати сторінкою за допомогою JavaScript, а також про асинхронність у JavaScript.</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>DOM Basics, DOM Styling and Sizing, Events, Promises, Portfolio Project</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>React</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Реактивненько вриваємось у світ фреймворків та UI-бібліотек. Прийшов час познайомитися з однією з найпопулярніших бібліотек у фронтенд-розробці. У цьому модулі ти дізнаєшся, що таке компонентний підхід до розробки, а також розробиш перший інтерактивний інтерфейс та створиш роботу для портфоліо!</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Props, Rendering Lists, Handling Events, List Manipulation, Lifting State Up, Updating State</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>TypeScript</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript ми вже знаємо. Прийшла черга зробити наш код більш передбачуваним і безпечним, а розробку приємнішою. У цьому модулі ти дізнаєшся, що таке статична типізація й чим корисний TypeScript для розробника.</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Basic Types, Advanced Types, Object Types, Classes, Generic Types</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>React with TypeScript</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти познайомишся з магією TypeScript у React.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Forms, Advanced Hooks, Component Lifecycle, Custom Hooks, Loading Data From API, Updating Data on Server, State Management, React Router, Working With URLSearchParams, Portfolio</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Redux</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Що там по менеджменту? Розберемось, як використовувати бібліотеку Redux в парі з бібліотекою React для менеджменту загального стану твого додатка. Припинимо прокидатися в холодному поту від слова «ред'юсер». Або почнемо…</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, React Redux, Async Redux</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>How the Web Works</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Кожного дня ти так чи інакше взаємодієш із мережею Інтернет. Але чи замислювався ти над тим, як працює всесвітня павутина? У цьому модулі ми допоможемо тобі розібратися з тим, як взаємодіють та обмінюються даними наші пристрої в мережі та що таке Інтернет в цілому.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to the Web, OSI Model, HTTP, API Interface, Encryption, Security in the Web</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>SQL Basics</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Node.js</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Ну що, frontend вже підкорений? Тоді саме час почати писати сервери на Javascript! У цьому модулі ти зануришся у світ Node.js і backend-розробки, дізнаєшся як створити API та авторизувати користувача. Також ти будеш працювати з базою даних і WebSocket, писати тести, деплоїти проєкти та багато чого іншого.</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Modules, Development Environment, Working With Command Line, Working With Files, HTTP Module, Event Loop, Streams, Express, Working With Databases, Node.js App Deployment, Authentication, Realtime Applications</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Tech Interview</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ми розглянемо важливі теми для проходження технічної співбесіди, які залишилися поза курсом.</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Final Portfolio Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Vue.js</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти створиш додаток ToDo за допомогою фреймворку Vue.js, використовуючи його систему реактивності, компоненти та обробку даних за допомогою Axios. Ти також вивчиш передові методи та розгорнеш свій додаток на GitHub Pages.</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>TodoApp with Vue.js</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Angular</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Angular — це популярний JS-фреймворк для створення масштабованих односторінкових вебдодатків. У цьому модулі ти вивчиш концепції Angular, від основ і структури проєкту до складних тем, таких як форми, компоненти, спостережувані параметри, управління станом, обробка помилок і оптимізація продуктивності.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Angular Basics</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Алгоритми замовляли? У цьому модулі ми познайомимося з різними структурами даних та алгоритмами. Навчимося обходити дерева краще сина маминої подруги, сортувати масиви зі швидкістю quick sort, створювати hash map та не тільки стояти в черзі, а й реалізовувати її. І це тільки маленька частинка того, що тебе чекає в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Main Concepts, Algorithm Complexity, Data Structures: Array, Search Algorithms, Data Structures: Linked List, Data Structures: Stack, Data Structures: Queue, Data Structures: Hash Map, Data Structures: Hash Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>Object Oriented Programming</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>На технічній співбесіді початківців часто запитують про Об'єктно-орієнтоване програмування (ООП) та його основні принципи.
+У цьомо модулі ти познайомишся з основами ООП та іншими речами, про які тебе можуть запитати.</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Basic Principles, SOLID Principles</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>JavaScript Testing</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Тестування — це важливо! Але чим більше коду, тим більше треба перевіряти кожного разу. Автоматизація дозволить значно спростити цей процес.</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to Javascript Automated Testing, Unit Testing, TDD Basics, Mock Basics, Advanced Mocks, Cypress</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Career Development</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль спрямований на розвиток навичок, необхідних для досягнення успіху в професійній сфері, а саме: стратегії кар'єрного зростання, важливі аспекти особистісного розвитку та інструменти для досягнення професійних цілей.</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Mastering Your Probation Period, PDP and Career Plans, Salary Review Strategies, Recruiter Outreach, How to Find a New Job?</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>DevOps Basics</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>У цьому модулі ти розглянеш як організована розробка програмного забезпечення та як її можна оптимізувати. А найголовніше — яка роль DevOps-інженера в усьому цьому.</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, DevOps Culture and Practices, DevOps as a Role, SDLC and Development Methodologies, Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>Docker Core</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Саме час познайомитись із технологією контейнеризації та Docker — де-факто стандартом для розповсюдження та запуску вебзастосунків. Тож, уперед!</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Docker Setup, Docker Introduction, Docker Internals, Docker Basics, Containerizing an App, Managing Containers, Docker Volumes, Docker Compose, 12-Factor App</t>
         </is>
       </c>
     </row>
@@ -2109,7 +3572,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2117,7 +3580,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="33" customWidth="1" min="1" max="1"/>
+    <col width="49" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
@@ -2258,6 +3721,227 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>SQL Basics</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>У рамках даного модуля ти познайомишся з поняттям бази даних, а також дізнаєшся, які існують види баз даних. Ти розглянеш, яким чином зберігається інформація в реляційних базах, та навчишся писати запити SELECT, щоб отримувати потрібну інформацію в бажаному вигляді. Після завершення модуля ти будеш знати, що таке INNER JOIN та для чого він використовується, будеш вміти сортувати та групувати дані за потрібними критеріями, а також застосовувати різні функції конкретної БД. Отож, поїхали!</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Introduction to SQL, SELECT Statement, WHERE Statement, NULL Value, LIKE, BETWEEN, and IN Statements, ORDER BY, LIMIT, DISTINCT, Aliases, Aggregate Functions, GROUP BY Statement, JOIN Statement, Functions, HAVING Statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Python Core for DevOps</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Ось і настав час заглибитись у світ Python Core і прокачатися як розробник. У цьому модулі ти використаєш знання на практиці, а генератори, ітератори та декоратори перестануть тебе лякати.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>How to Solve GitHub Tasks, Mutable Immutable Types, List and Dict Comprehensions, Functions in Details, Decorators, Classes, Сlasses in Details, Iterators and Generators, Modules and Imports, Exception Handling, Exceptions in Details, File Handling, Testing, Testing in Details, FastAPI Overview, FastAPI in Details</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Docker Core</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Саме час познайомитись із технологією контейнеризації та Docker — де-факто стандартом для розповсюдження та запуску вебзастосунків. Тож, уперед!</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Docker Setup, Docker Introduction, Docker Internals, Docker Basics, Containerizing an App, Managing Containers, Docker Volumes, Docker Compose, 12-Factor App</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Relational Database Administration</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Тепер, коли ти вмієш користуватись базами даних, саме час дізнатись як керувати власним сервером для них. А найголовніше — як робити бекап бази даних!</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Database Intro, Database Design Fundamentals, Database Design Advanced, Database Internals, Configuring the Database, Running Database Migrations, Monitoring Database Server, Backup and Restoration, Replication</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Kubernetes Basics</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Запустити один контейнер доволі просто. Але що робити, якщо їх сотні? У цьому модулі ти освоїш платформу Kubernetes, яка допоможе розв'язати цю проблему.</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Module Overview, Kubernetes Introduction, Kubernetes Architecture, Lab SetUp, Working With Pods, Working With Services, Controllers and Deployments, DeamonSets and Jobs, Configuration Management, Storage and StatefulSets, Cluster Networking: Ingress, Scheduling in Details, Helm  Architecture, RBAC and Service Accounts, Helm Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Monitoring and Observability</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Чи задоволені користувачі твого веб сервісу? Єдиний спосіб на це відповісти - мати правильно сконфігурований моніторинг, і цей модуль допоможе тобі розібратись, як саме це зробити.</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Module Overview, Monitoring and Observability, Monitoring Tools Overview, Prometheus-Like Monitoring (Instrumenting App), Alerting, Grafana Dashboards, Monitoring Kubernetes, Monitoring Techniques</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Cloud Computing Basics</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Хмарні технології дозволяють запускати код у будь-якій частині світу та розширювати інфраструктуру з одного серверу до сотні всього в кілька кліків. Настав час розглянути ці можливості.</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Module Overview, Environment Setup, Main Concepts, Azure Overview, Azure Virtual Machine Basics, Azure PowerShell, Azure Virtual Machine Advanced, Automating Resource Deployment With Azure Resource Manager (ARM) Templates, Managing Users and Groups in Microsoft Entra ID, Managing Access to Azure Resources</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>DevOps Practices: CI/CD</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>CI/CD — це серце циклу розробки програмного забезпечення. Тут ти навчишся будувати цей процес розробки та автоматизовувати його за допомогою GitHub Actions.</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Module Overview, Introduction to CI/CD and GitHub Actions, GitHub Actions: CI for Python app, GitHub Actions: CI for Docker, GitHub Actions: CI for Helm, GitHub Actions CD: Azure Kubernetes Services, Polishing Workflow</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Infrastructure as a Code With Terraform</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Що означає «Infrastructure as a Code», які переваги має цей підхід та як створити хмарну інфраструктуру за допомогою Terraform? Усе це ми розглянемо в цьому модулі.</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Terraform State, HCL Language Features, Terraform Provisioners, Working with Terraform, Getting Started with Terraform, Introduction to Infrastructure as Code, Portfolio Project, Module Overview, Terraform Modules</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Employment</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Відшліфовуємо резюме, рекомендаційний лист та профілі в професійних соціальних мережах. Працюємо з базою вакансій. Проходимо тестові технічні та нетехнічні інтерв’ю. Вчимося комунікувати з рекрутерами. Проходимо справжнє інтерв’ю. Приймаємо оффер. Виходимо на роботу.</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Introduction, Preparing Your Resume, Interview Preparation, Preparing Your Cover Letter, DOU and Google Profiles, Creating Your LinkedIn Profile, How to Communicate in the Right Way, Creating Your Djinni Profile, How to Find Vacancies, How to Apply for a Job on Different Platforms, How to Find Recruiters' Contacts, Employment Daily Activities, Work Details FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Cloud Computing Extended</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Azure — одна з найпопулярніших хмарних платформ. Тож розглянемо її та навчимось працювати з базовими сервісами.</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Module Overview, Azure Virtual Networks Overview, Configure Secure Access to Virtual Networks, Configure Name Resolution in Virtual Networks, Configure Load Balancing, Web Apps</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Other DevOps Practices</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Цей модуль ознайомить тебе з додатковими практиками та підходами DevOps, які дозволять ще ефективніше будувати процеси для розробки програмного забезпечення.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Incident Comand System, Immutable infrastructure, Chaos engineering, Deployment strategies, Dependency injection, Blameless postmortems, Status pages, Developers on call, SRE practices, DevOps antipatterns, Chatops</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Architecture Patterns &amp; Reference Architectures</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Архітектура — це спосіб організації компонентів системи або програми. Розробники підходять до цього по-різному, але декілька таких підходів вирізняються популярністю. У цьому модулі ми їх і розглянемо.</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Replication, Queue, HA &amp; DR, Microservices, SOLID, Service discovery, Clustering, Monolith</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>